<commit_message>
relatório + update dos prints
</commit_message>
<xml_diff>
--- a/Use Cases - Atendimento a Clientes.xlsx
+++ b/Use Cases - Atendimento a Clientes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ambrosiny/Desktop/Universidade/3ano/DSS/Trabalho_DSS/dss-projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MIEI\3º Ano\1º Semestre\Desenvolvimento de Sistemas de Software\Projeto\dss-projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0510EE78-A4E0-4B79-82B7-4DBE18B805A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="2880" windowWidth="38400" windowHeight="21600" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="9180" yWindow="2880" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adiciona Componente" sheetId="2" r:id="rId1"/>
@@ -39,38 +40,12 @@
     <t>4.2.2. Informa que a seleção foi cancelada</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">4.2.1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t>Recusa instalar componentes necessários</t>
-    </r>
-  </si>
-  <si>
     <t>Cenário 
 Excepção 3  
 [cancela a seleção] (passo 4.2)</t>
   </si>
   <si>
     <t xml:space="preserve">3.2.2. Informa que a seleção foi cancelada </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3.2.1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t>Recusa remover componente incompatível</t>
-    </r>
   </si>
   <si>
     <t>Cenário 
@@ -496,12 +471,18 @@
   <si>
     <t>2. Apresenta dados sobre a configuração</t>
   </si>
+  <si>
+    <t>3.2.1. Recusa remover componente incompatível</t>
+  </si>
+  <si>
+    <t>4.2.1. Recusa instalar componentes necessários</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,11 +496,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri (Corpo)"/>
     </font>
     <font>
       <sz val="12"/>
@@ -814,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -822,9 +798,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -840,52 +813,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -925,20 +865,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,15 +890,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -977,11 +908,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1262,208 +1229,208 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="54.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="36.375" customWidth="1"/>
+    <col min="4" max="4" width="54.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="16.5" thickBot="1">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="24" t="s">
+    <row r="2" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B2" s="49" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+      <c r="C2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="54"/>
-    </row>
-    <row r="4" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+    </row>
+    <row r="3" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B3" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C3" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="54"/>
-    </row>
-    <row r="5" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="D3" s="50"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="54"/>
-    </row>
-    <row r="6" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+      <c r="D4" s="50"/>
+    </row>
+    <row r="5" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B5" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D5" s="50"/>
+    </row>
+    <row r="6" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B6" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="56"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="19" t="s">
+      <c r="C6" s="52" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
-      <c r="C8" s="18" t="s">
+      <c r="D6" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="2:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="57"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="6" t="s">
+    </row>
+    <row r="7" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B7" s="41"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="6" t="s">
+    <row r="8" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B8" s="41"/>
+      <c r="C8" s="56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="6" t="s">
+      <c r="D8" s="57"/>
+    </row>
+    <row r="9" spans="2:5" ht="45" customHeight="1" thickBot="1">
+      <c r="B9" s="41"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="57"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="6" t="s">
+    <row r="10" spans="2:5" ht="43.5" customHeight="1" thickBot="1">
+      <c r="B10" s="41"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="38" x14ac:dyDescent="0.2">
-      <c r="B13" s="50" t="s">
+    <row r="11" spans="2:5" ht="19.5" thickBot="1">
+      <c r="B11" s="41"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5" t="s">
+    </row>
+    <row r="12" spans="2:5" ht="63.75" customHeight="1" thickBot="1">
+      <c r="B12" s="41"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:5" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="52"/>
-      <c r="C14" s="16"/>
+    </row>
+    <row r="13" spans="2:5" ht="37.5">
+      <c r="B13" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" ht="64.5" customHeight="1" thickBot="1">
+      <c r="B14" s="40"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="B16" s="51"/>
-      <c r="C16" s="15" t="s">
+    <row r="15" spans="2:5" ht="38.25" customHeight="1">
+      <c r="B15" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="2:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="52"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="12" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="50" t="s">
+    <row r="16" spans="2:5" ht="18.75">
+      <c r="B16" s="39"/>
+      <c r="C16" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10" t="s">
+      <c r="D16" s="59"/>
+    </row>
+    <row r="17" spans="2:6" ht="47.25" customHeight="1" thickBot="1">
+      <c r="B17" s="40"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="51"/>
-      <c r="C19" s="9" t="s">
+    <row r="18" spans="2:6" ht="40.5" customHeight="1">
+      <c r="B18" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="8" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+    <row r="19" spans="2:6" ht="42" customHeight="1">
+      <c r="B19" s="39"/>
+      <c r="C19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B20" s="40"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="51"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6" t="s">
+    </row>
+    <row r="21" spans="2:6" ht="39.950000000000003" customHeight="1">
+      <c r="B21" s="38" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="50" t="s">
+      <c r="C21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="2:6" ht="45" customHeight="1" thickBot="1">
+      <c r="B22" s="39"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="5" t="s">
+    </row>
+    <row r="23" spans="2:6" ht="38.1" customHeight="1">
+      <c r="B23" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="52"/>
-      <c r="C24" s="3"/>
+      <c r="C23" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="2:6" ht="48" customHeight="1" thickBot="1">
+      <c r="B24" s="40"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1488,197 +1455,197 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="33.375" customWidth="1"/>
+    <col min="4" max="4" width="49.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="46"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="46"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="42"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="42"/>
+      <c r="C8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="42"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="42"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="2:4" ht="37.5">
+      <c r="B13" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:4" ht="87" customHeight="1" thickBot="1">
+      <c r="B14" s="40"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B15" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B16" s="44"/>
+      <c r="C16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="2:4" ht="45" customHeight="1" thickBot="1">
+      <c r="B17" s="44"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="39.75" customHeight="1" thickBot="1">
+      <c r="B18" s="44"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B19" s="44"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B20" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B21" s="44"/>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="2:4" ht="39.75" customHeight="1" thickBot="1">
+      <c r="B22" s="44"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B23" s="44"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="61"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="61"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="61"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="61"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="57"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="57"/>
-      <c r="C8" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="2:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B13" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="52"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="59"/>
-      <c r="C16" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="2:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="59"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="59"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="59"/>
-      <c r="C21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" spans="2:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="59"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="59"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="59"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="8" t="s">
-        <v>35</v>
+    </row>
+    <row r="24" spans="2:4" ht="26.25" customHeight="1" thickBot="1">
+      <c r="B24" s="44"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1697,203 +1664,203 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="61"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="61"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+    <row r="4" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="34" t="s">
+      <c r="C6" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="61"/>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56" t="s">
+      <c r="C7" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="32" t="s">
+      <c r="C8" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="46"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="27"/>
-    </row>
-    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
-      <c r="C13" s="26" t="s">
+      <c r="C9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="27" t="s">
+    </row>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="42"/>
+      <c r="C11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B12" s="42"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="31" t="s">
+    <row r="13" spans="2:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B13" s="42"/>
+      <c r="C13" s="14" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
-      <c r="C16" s="29" t="s">
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="42"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="57"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="27" t="s">
+    </row>
+    <row r="15" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B15" s="42"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="56" t="s">
+    <row r="16" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B16" s="42"/>
+      <c r="C16" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B17" s="42"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="2:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="57"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="6" t="s">
+    </row>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B18" s="42"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B19" s="41" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="56" t="s">
+      <c r="C19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="2:4" ht="79.5" customHeight="1" thickBot="1">
+      <c r="B20" s="42"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="35"/>
-    </row>
-    <row r="22" spans="2:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="57"/>
-      <c r="C22" s="25"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B21" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="23"/>
+    </row>
+    <row r="22" spans="2:4" ht="66" customHeight="1" thickBot="1">
+      <c r="B22" s="42"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="45" t="s">
+    </row>
+    <row r="23" spans="2:4" ht="42" customHeight="1" thickBot="1">
+      <c r="B23" s="47" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="62"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="47" t="s">
+      <c r="C23" s="32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="63"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="36" t="s">
+      <c r="D23" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="35"/>
-    </row>
-    <row r="27" spans="2:4" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="57"/>
-      <c r="C27" s="25"/>
+    </row>
+    <row r="24" spans="2:4" ht="22.5" customHeight="1" thickBot="1">
+      <c r="B24" s="47"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="37.5" customHeight="1" thickBot="1">
+      <c r="B25" s="48"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B26" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="2:4" ht="83.25" customHeight="1" thickBot="1">
+      <c r="B27" s="42"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B23:B25"/>
@@ -1912,129 +1879,129 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="32.5" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="61"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="61"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+    <row r="4" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="34" t="s">
+      <c r="C6" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="61"/>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56" t="s">
+      <c r="C7" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="32" t="s">
+      <c r="C8" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="46"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="31" t="s">
+      <c r="C9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="27" t="s">
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="42"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="42"/>
+      <c r="C12" s="17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="56" t="s">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="42"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="36" t="s">
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="42"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="40"/>
-    </row>
-    <row r="17" spans="2:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="57"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="19" t="s">
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B15" s="42"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B16" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="38"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="G18" s="38"/>
+      <c r="C16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="2:7" ht="84" customHeight="1" thickBot="1">
+      <c r="B17" s="42"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="G18" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2050,88 +2017,88 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C4:E12"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C5" sqref="C5:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="61"/>
-    </row>
-    <row r="6" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="61"/>
-    </row>
-    <row r="7" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="34" t="s">
+    <row r="4" spans="3:5" ht="16.5" thickBot="1"/>
+    <row r="5" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="61"/>
-    </row>
-    <row r="8" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="34" t="s">
+      <c r="D6" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="61"/>
-    </row>
-    <row r="9" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="56" t="s">
+      <c r="D7" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="42" t="s">
+      <c r="D8" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="46"/>
+    </row>
+    <row r="9" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C9" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="57"/>
-      <c r="D10" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="57"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="57"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="37"/>
+      <c r="D9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="24.75" customHeight="1" thickBot="1">
+      <c r="C10" s="42"/>
+      <c r="D10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C11" s="42"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="19.5" thickBot="1">
+      <c r="C12" s="42"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2146,147 +2113,147 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" s="61"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="61"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
+    <row r="3" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="61"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+      <c r="C5" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56" t="s">
+      <c r="C6" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="32" t="s">
+      <c r="C7" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
-      <c r="C9" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="27"/>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="31" t="s">
+      <c r="C8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="26" t="s">
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="27" t="s">
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="42"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="57"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="27"/>
-    </row>
-    <row r="15" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="56" t="s">
+    <row r="12" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B12" s="42"/>
+      <c r="C12" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="40" t="s">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="42"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="41" t="s">
+    <row r="14" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B14" s="42"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="2:4" ht="22.5" customHeight="1" thickBot="1">
+      <c r="B15" s="41" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="56" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="36" t="s">
+    </row>
+    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1">
+      <c r="B16" s="42"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="35"/>
-    </row>
-    <row r="18" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="31" t="s">
+    </row>
+    <row r="17" spans="2:5" ht="38.25" customHeight="1" thickBot="1">
+      <c r="B17" s="41" t="s">
         <v>95</v>
       </c>
+      <c r="C17" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="2:5" ht="38.25" thickBot="1">
+      <c r="B18" s="42"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="E18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="57"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="37"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="23.1" customHeight="1" thickBot="1">
+      <c r="B19" s="42"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2303,112 +2270,112 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B3:D15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="29.375" customWidth="1"/>
+    <col min="4" max="4" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="61"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="61"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
+    <row r="3" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="61"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+      <c r="C5" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56" t="s">
+      <c r="C6" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="32" t="s">
+      <c r="C7" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
-      <c r="C9" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="27"/>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="35" t="s">
+      <c r="C8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="37"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B11" s="42"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="42"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="42"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1">
+      <c r="B14" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="63" customHeight="1" thickBot="1">
+      <c r="B15" s="42"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2424,120 +2391,120 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B3:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B4" sqref="B4:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.625" customWidth="1"/>
+    <col min="4" max="4" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="61"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="60" t="s">
+    <row r="3" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B8" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B9" s="42"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B10" s="42"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="38.25" thickBot="1">
+      <c r="B11" s="42"/>
+      <c r="C11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B12" s="42"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1">
+      <c r="B13" s="42"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1">
+      <c r="B14" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="28"/>
+    </row>
+    <row r="15" spans="2:4" ht="64.5" customHeight="1" thickBot="1">
+      <c r="B15" s="42"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="61"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="61"/>
-    </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="61"/>
-    </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="57"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="57"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="57"/>
-      <c r="C11" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="27"/>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="57"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="57"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="40"/>
-    </row>
-    <row r="15" spans="2:4" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Falta add comp e add pacote
</commit_message>
<xml_diff>
--- a/Use Cases - Atendimento a Clientes.xlsx
+++ b/Use Cases - Atendimento a Clientes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ambrosiny/Desktop/Universidade/3ano/DSS/Trabalho_DSS/dss-projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroferreira/Desktop/DSS/dss-projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="3580" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Adiciona Componente" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="113">
   <si>
     <t>4.2.2. Informa que a seleção foi cancelada</t>
   </si>
@@ -301,46 +301,10 @@
     <t>Consultar cliente</t>
   </si>
   <si>
-    <t>o</t>
-  </si>
-  <si>
     <t>4.2. Informa que o cliente não pode ser adicionado</t>
   </si>
   <si>
     <t>4.1. Não preenche todos os campos</t>
-  </si>
-  <si>
-    <t>Cenário 
-Excepção 2 
-[campos por preencher] 
-(passo 4)</t>
-  </si>
-  <si>
-    <t>2.2. Cancela registo</t>
-  </si>
-  <si>
-    <t>2.1. Informa que o cliente já existe</t>
-  </si>
-  <si>
-    <t>Cenário 
-Excepção 1 
-[cliente já existe] 
-(passo 2)</t>
-  </si>
-  <si>
-    <t>5. Adiciona o cliente</t>
-  </si>
-  <si>
-    <t>4. Preenche os dados do novo cliente</t>
-  </si>
-  <si>
-    <t>3. Mostra os campos com os dados a preencher</t>
-  </si>
-  <si>
-    <t>2. Verifica se o cliente já existe</t>
-  </si>
-  <si>
-    <t>1. Indica o cliente que vai ser adicionado</t>
   </si>
   <si>
     <t>Cliente adicionado à base de dados</t>
@@ -414,9 +378,6 @@
  (passo 3)</t>
   </si>
   <si>
-    <t>4. Identifica o cliente</t>
-  </si>
-  <si>
     <t>2. Apresenta lista de todos os clientes</t>
   </si>
   <si>
@@ -433,6 +394,33 @@
   </si>
   <si>
     <t>4. Regista encomenda</t>
+  </si>
+  <si>
+    <t>1. Indica que pretende adicionar um cliente</t>
+  </si>
+  <si>
+    <t>3. Preenche os dados do novo cliente</t>
+  </si>
+  <si>
+    <t>4. Adiciona o cliente</t>
+  </si>
+  <si>
+    <t>5. Informa que cliente foi adicionado</t>
+  </si>
+  <si>
+    <t>2. Pede para inserir dados relativos ao cliente</t>
+  </si>
+  <si>
+    <t>Cenário 
+Excepção 2 
+[dados por inserir] 
+(passo 4)</t>
+  </si>
+  <si>
+    <t>4. Obtém dados do cliente pretendido</t>
+  </si>
+  <si>
+    <t>5. Apresenta dados do cliente</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D21" s="8"/>
     </row>
@@ -1353,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D23" s="8"/>
     </row>
@@ -1665,7 +1653,7 @@
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52"/>
       <c r="C11" s="14" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D11" s="15"/>
     </row>
@@ -1673,14 +1661,14 @@
       <c r="B12" s="52"/>
       <c r="C12" s="17"/>
       <c r="D12" s="15" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="52"/>
       <c r="C13" s="17"/>
       <c r="D13" s="19" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -1796,14 +1784,14 @@
       <c r="B10" s="52"/>
       <c r="C10" s="17"/>
       <c r="D10" s="15" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52"/>
       <c r="C11" s="17"/>
       <c r="D11" s="5" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -1817,7 +1805,7 @@
       <c r="B13" s="52"/>
       <c r="C13" s="17"/>
       <c r="D13" s="19" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -1963,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E19"/>
+  <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1982,7 +1970,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D4" s="51"/>
     </row>
@@ -2000,7 +1988,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D6" s="51"/>
     </row>
@@ -2009,7 +1997,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D7" s="51"/>
     </row>
@@ -2027,92 +2015,67 @@
     <row r="9" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="52"/>
       <c r="C9" s="14" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="52"/>
       <c r="C10" s="17"/>
-      <c r="D10" s="15" t="s">
-        <v>86</v>
+      <c r="D10" s="19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="52"/>
-      <c r="C12" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="15"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="15" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="52"/>
       <c r="C13" s="17"/>
       <c r="D13" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="52"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="52"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="52"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="23"/>
-    </row>
-    <row r="18" spans="2:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="52"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="25"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B17:B19"/>
+  <mergeCells count="6">
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B8:B14"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B8:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2123,7 +2086,7 @@
   <dimension ref="B3:D15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2139,7 +2102,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D4" s="51"/>
     </row>
@@ -2157,7 +2120,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D6" s="51"/>
     </row>
@@ -2166,7 +2129,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D7" s="51"/>
     </row>
@@ -2185,20 +2148,20 @@
       <c r="B9" s="52"/>
       <c r="C9" s="17"/>
       <c r="D9" s="15" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="52"/>
       <c r="C10" s="17"/>
       <c r="D10" s="15" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52"/>
       <c r="C11" s="17" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D11" s="15"/>
     </row>
@@ -2206,20 +2169,22 @@
       <c r="B12" s="52"/>
       <c r="C12" s="17"/>
       <c r="D12" s="15" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="52"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="47" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D14" s="23"/>
     </row>
@@ -2227,7 +2192,7 @@
       <c r="B15" s="52"/>
       <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2245,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D28"/>
+  <dimension ref="B3:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2264,7 +2229,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D4" s="51"/>
     </row>
@@ -2291,7 +2256,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D7" s="51"/>
     </row>
@@ -2317,13 +2282,13 @@
       <c r="B10" s="52"/>
       <c r="C10" s="17"/>
       <c r="D10" s="15" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52"/>
       <c r="C11" s="14" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D11" s="15"/>
     </row>
@@ -2331,43 +2296,38 @@
       <c r="B12" s="52"/>
       <c r="C12" s="17"/>
       <c r="D12" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="52"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="2:4" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="52"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="2:4" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="52"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>